<commit_message>
We add Amazon sample and test results
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDriveFolderBis\OneDrive\Serginet Startup\Repos\ServerlessWars\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/331d9f6799ea1c34/Serginet Startup/Repos/ServerlessWars/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BED21B06-7863-4FCE-BF0C-61FD48DF361C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{15046972-54B1-43ED-A5D3-01AE047717F4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{C0A6BD0B-E716-4739-9F3F-5E6DB94E2669}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$2:$N$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$2:$N$21</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
   <si>
     <t>Platform</t>
   </si>
@@ -443,11 +443,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246999E2-8D6C-4DC8-ADE1-427EFC9D9FF8}">
-  <dimension ref="B2:N18"/>
+  <dimension ref="B2:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1053,7 +1051,7 @@
         <v>16</v>
       </c>
       <c r="F16">
-        <v>150</v>
+        <v>25</v>
       </c>
       <c r="G16">
         <v>500</v>
@@ -1061,8 +1059,26 @@
       <c r="H16">
         <v>12500</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>93</v>
+      </c>
+      <c r="J16">
+        <v>118</v>
+      </c>
+      <c r="K16">
+        <v>1877</v>
+      </c>
+      <c r="L16">
+        <v>166</v>
+      </c>
+      <c r="M16">
+        <v>43.97</v>
+      </c>
+      <c r="N16">
+        <v>133.69999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1076,7 +1092,7 @@
         <v>16</v>
       </c>
       <c r="F17">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="G17">
         <v>500</v>
@@ -1084,8 +1100,26 @@
       <c r="H17">
         <v>25000</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>95</v>
+      </c>
+      <c r="J17">
+        <v>118</v>
+      </c>
+      <c r="K17">
+        <v>1586</v>
+      </c>
+      <c r="L17">
+        <v>171</v>
+      </c>
+      <c r="M17">
+        <v>50.6</v>
+      </c>
+      <c r="N17">
+        <v>260.8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1107,9 +1141,150 @@
       <c r="H18">
         <v>75000</v>
       </c>
+      <c r="I18">
+        <v>109</v>
+      </c>
+      <c r="J18">
+        <v>118</v>
+      </c>
+      <c r="K18">
+        <v>2502</v>
+      </c>
+      <c r="L18">
+        <v>196</v>
+      </c>
+      <c r="M18">
+        <v>79.569999999999993</v>
+      </c>
+      <c r="N18">
+        <v>683.2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19">
+        <v>25</v>
+      </c>
+      <c r="G19">
+        <v>500</v>
+      </c>
+      <c r="H19">
+        <v>12500</v>
+      </c>
+      <c r="I19">
+        <v>73</v>
+      </c>
+      <c r="J19">
+        <v>115</v>
+      </c>
+      <c r="K19">
+        <v>1167</v>
+      </c>
+      <c r="L19">
+        <v>127</v>
+      </c>
+      <c r="M19">
+        <v>31.58</v>
+      </c>
+      <c r="N19">
+        <v>169.7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20">
+        <v>50</v>
+      </c>
+      <c r="G20">
+        <v>500</v>
+      </c>
+      <c r="H20">
+        <v>25000</v>
+      </c>
+      <c r="I20">
+        <v>74</v>
+      </c>
+      <c r="J20">
+        <v>114</v>
+      </c>
+      <c r="K20">
+        <v>950</v>
+      </c>
+      <c r="L20">
+        <v>129</v>
+      </c>
+      <c r="M20">
+        <v>36.24</v>
+      </c>
+      <c r="N20">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21">
+        <v>150</v>
+      </c>
+      <c r="G21">
+        <v>500</v>
+      </c>
+      <c r="H21">
+        <v>75000</v>
+      </c>
+      <c r="I21">
+        <v>84</v>
+      </c>
+      <c r="J21">
+        <v>114</v>
+      </c>
+      <c r="K21">
+        <v>1998</v>
+      </c>
+      <c r="L21">
+        <v>141</v>
+      </c>
+      <c r="M21">
+        <v>66.73</v>
+      </c>
+      <c r="N21">
+        <v>885.9</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:N18" xr:uid="{E22C4B8F-04F2-4800-8D65-434B9D70256C}"/>
+  <autoFilter ref="B2:N21" xr:uid="{E22C4B8F-04F2-4800-8D65-434B9D70256C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>